<commit_message>
Add new hardware CAD files and update BOM
Added several new Inventor assembly and part files for A4988 driver, Arduino Mega 2560, magnetometer holder, and related assemblies. Updated and added historical versions in OldVersions. Modified existing assemblies and BOM_list.xlsx. Added new price screenshots and related planning documents.
</commit_message>
<xml_diff>
--- a/planning/BOM_list.xlsx
+++ b/planning/BOM_list.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schar\Desktop\projectBlueprint\AMSTS\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6DD1B0-1D46-462B-BD7F-DD32CA01ABF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984AEA46-175C-4A38-8DFF-492F261E7B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="361" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="361" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="Cost" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="230">
   <si>
     <t>Item</t>
   </si>
@@ -648,19 +649,107 @@
   </si>
   <si>
     <t>Buy - Produce</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Seller</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>4x2020_raw</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>manual_locker_raw</t>
+  </si>
+  <si>
+    <t>manual_locker_upper_raw</t>
+  </si>
+  <si>
+    <t>AMT222D-V</t>
+  </si>
+  <si>
+    <t>AMT-06C-1-036</t>
+  </si>
+  <si>
+    <t>Adafruit 6109 (A4988)</t>
+  </si>
+  <si>
+    <t>Arduino MEGA 2560 A000067</t>
+  </si>
+  <si>
+    <t>Mouser Electronics GmbH</t>
+  </si>
+  <si>
+    <t>eu.mouser.com</t>
+  </si>
+  <si>
+    <t>Subsum for Seller:</t>
+  </si>
+  <si>
+    <t>Blexon AG</t>
+  </si>
+  <si>
+    <t>blexon.com</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>8000mm 2020 Profile</t>
+  </si>
+  <si>
+    <t>eBay</t>
+  </si>
+  <si>
+    <t>NEMA 17 1:50 PG</t>
+  </si>
+  <si>
+    <t>NEMA 17 Stepper Motors</t>
+  </si>
+  <si>
+    <t>https://www.omc-stepperonline.com/</t>
+  </si>
+  <si>
+    <t>StepperMotors</t>
+  </si>
+  <si>
+    <t>Sum:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -689,10 +778,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -704,8 +794,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3970,8 +4067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="C63" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5816,4 +5913,365 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{635A1669-18AD-40E9-B2D7-43EDF5373F41}">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.26953125" customWidth="1"/>
+    <col min="2" max="2" width="25.90625" customWidth="1"/>
+    <col min="3" max="3" width="6.36328125" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="28.6328125" customWidth="1"/>
+    <col min="6" max="6" width="43.90625" customWidth="1"/>
+    <col min="8" max="8" width="20.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2" s="7">
+        <v>72.790000000000006</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="I4" s="7">
+        <v>109.87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>44.77</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>29.52</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" s="7">
+        <v>11.96</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
+        <v>38.33</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="I8" s="7">
+        <f>SUM(D5:D8)</f>
+        <v>124.58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9" s="8">
+        <v>78.56</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" s="8">
+        <v>67.89</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="F10" t="s">
+        <v>227</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" s="8">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="F11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8">
+        <v>22.99</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="D15" s="7">
+        <f>SUM(D2:D12)</f>
+        <v>385.41</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="E19" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F9" r:id="rId1" xr:uid="{6BB673A0-D5B9-43BD-8EE0-E9BFBE6F2CF5}"/>
+    <hyperlink ref="F12" r:id="rId2" xr:uid="{0E085989-D197-4AE4-B7FE-119AE89FA0FE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>